<commit_message>
updated reference database information
</commit_message>
<xml_diff>
--- a/databases/20221113-phyloassigner_DB_context_CJC.xlsx
+++ b/databases/20221113-phyloassigner_DB_context_CJC.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28705"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fwittmers/Documents/GitHub/PhyloAssigner_python_UCSB/databases/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40EAA26E-44AA-9B49-BB25-2CD33CD70381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="0" windowWidth="23240" windowHeight="19720" tabRatio="864" activeTab="6"/>
+    <workbookView xWindow="400" yWindow="760" windowWidth="23240" windowHeight="19720" tabRatio="864" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="16S_CyanoPlastid" sheetId="1" r:id="rId1"/>
@@ -15,13 +21,13 @@
     <sheet name="16S_Cyanobacteria" sheetId="8" r:id="rId6"/>
     <sheet name="16S_Pelagophytes" sheetId="5" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -390,9 +396,6 @@
     <t>Apedinella</t>
   </si>
   <si>
-    <t>Chattonella</t>
-  </si>
-  <si>
     <t>Dictyocha</t>
   </si>
   <si>
@@ -2970,13 +2973,16 @@
   </si>
   <si>
     <t>FC-III</t>
+  </si>
+  <si>
+    <t>Pseudochattonella</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="17" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="17">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3122,13 +3128,12 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3137,7 +3142,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -3462,80 +3466,80 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView zoomScale="115" workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="14.83203125" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
     <col min="3" max="3" width="60.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="10" customFormat="1" ht="24" customHeight="1">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:6" s="9" customFormat="1" ht="24" customHeight="1">
+      <c r="A1" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="17">
+      <c r="C1" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="18">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3" spans="1:6" ht="17">
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:6" ht="18">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="17">
+    </row>
+    <row r="4" spans="1:6" ht="18">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:6" ht="17">
+    <row r="5" spans="1:6" ht="18">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:6" ht="17">
+    <row r="6" spans="1:6" ht="18">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -3544,136 +3548,136 @@
       </c>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:6" ht="17">
+    <row r="7" spans="1:6" ht="18">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="F7" s="7"/>
-    </row>
-    <row r="8" spans="1:6" ht="17">
+        <v>191</v>
+      </c>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:6" ht="19">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D8" s="12"/>
-    </row>
-    <row r="9" spans="1:6" ht="17">
+        <v>191</v>
+      </c>
+      <c r="D8" s="11"/>
+    </row>
+    <row r="9" spans="1:6" ht="18">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="17">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="18">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="7"/>
-    </row>
-    <row r="11" spans="1:6" ht="17">
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:6" ht="18">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="17">
+    </row>
+    <row r="12" spans="1:6" ht="18">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="17">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="18">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="17">
+    </row>
+    <row r="14" spans="1:6" ht="18">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="17">
+    </row>
+    <row r="15" spans="1:6" ht="18">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:6" ht="17">
+    <row r="16" spans="1:6" ht="18">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="17">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="18">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="17">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="18">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="1:3" ht="17">
+    <row r="19" spans="1:3" ht="18">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
@@ -3682,7 +3686,7 @@
       </c>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="1:3" ht="17">
+    <row r="20" spans="1:3" ht="18">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
@@ -3703,14 +3707,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="2" width="47.1640625" customWidth="1"/>
@@ -3719,21 +3723,21 @@
     <col min="5" max="5" width="137.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="10" customFormat="1" ht="24" customHeight="1">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:6" s="9" customFormat="1" ht="24" customHeight="1">
+      <c r="A1" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="E1" s="8" t="s">
+      <c r="C1" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>198</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16" customHeight="1">
@@ -3741,192 +3745,185 @@
         <v>19</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C2" t="s">
         <v>185</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="E2" s="13"/>
+      <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>186</v>
+      </c>
+      <c r="C3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="19">
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="C4" s="5"/>
+        <v>160</v>
+      </c>
       <c r="D4" t="s">
-        <v>201</v>
-      </c>
-      <c r="E4" s="12" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="E4" s="11" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="19">
       <c r="A5" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="C5" s="5"/>
+        <v>179</v>
+      </c>
       <c r="D5" t="s">
-        <v>203</v>
-      </c>
-      <c r="E5" s="12" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="E5" s="11" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="19">
       <c r="A6" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="C6" s="14"/>
+        <v>181</v>
+      </c>
+      <c r="C6" s="6"/>
       <c r="D6" t="s">
-        <v>201</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>200</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="19">
       <c r="A7" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>183</v>
+        <v>180</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>182</v>
       </c>
       <c r="D7" t="s">
-        <v>203</v>
-      </c>
-      <c r="E7" s="12" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="E7" s="11" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="19">
       <c r="A8" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C8" t="s">
         <v>178</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="D8" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" ht="19">
       <c r="A9" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>183</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="19">
       <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="D10" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="19">
       <c r="A11" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="D11" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="19">
       <c r="A12" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="D12" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="19">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="D13" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="19">
       <c r="A14" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>207</v>
+      <c r="D14" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -3936,9 +3933,8 @@
       <c r="B15" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="17" t="s">
-        <v>201</v>
+      <c r="D15" s="15" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -3946,220 +3942,206 @@
         <v>33</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="17" t="s">
-        <v>201</v>
+        <v>161</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="17" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="B17" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="19">
       <c r="A18" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>163</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="19">
       <c r="A19" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>168</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="19">
       <c r="A20" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>175</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="19">
       <c r="A21" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="C21" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="D21" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="C21" t="s">
+        <v>173</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="19">
       <c r="A22" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="E22" s="18" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+        <v>170</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="19">
       <c r="A23" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+        <v>172</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="19">
       <c r="A24" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>171</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="19">
       <c r="A25" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+        <v>153</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="19">
       <c r="A26" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+        <v>153</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="19">
       <c r="A27" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+        <v>154</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="19">
       <c r="A28" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B28" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="B28" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="19">
       <c r="A29" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B29" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="B29" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="19">
       <c r="A30" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>215</v>
+        <v>169</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -4167,11 +4149,10 @@
         <v>48</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="17" t="s">
-        <v>201</v>
+        <v>157</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -4179,115 +4160,109 @@
         <v>49</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="17" t="s">
-        <v>201</v>
+        <v>158</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B33" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="17" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="B33" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="19">
       <c r="A34" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="C34" s="5"/>
-      <c r="D34" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="E34" s="12" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+        <v>176</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="19">
       <c r="A35" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="E35" s="12" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+        <v>165</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="19">
       <c r="A36" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C36" s="16"/>
-      <c r="D36" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+        <v>166</v>
+      </c>
+      <c r="C36" s="14"/>
+      <c r="D36" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="19">
       <c r="A37" s="3" t="s">
         <v>54</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C37" t="s">
+        <v>167</v>
+      </c>
+      <c r="D37" t="s">
+        <v>200</v>
+      </c>
+      <c r="E37" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="C37" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="D37" t="s">
-        <v>201</v>
-      </c>
-      <c r="E37" s="12" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+    </row>
+    <row r="38" spans="1:5" ht="19">
       <c r="A38" s="3" t="s">
         <v>55</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C38" s="5"/>
       <c r="D38" t="s">
-        <v>203</v>
-      </c>
-      <c r="E38" s="12" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+        <v>202</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="19">
       <c r="A39" s="3" t="s">
         <v>56</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C39" s="5"/>
       <c r="D39" t="s">
-        <v>203</v>
-      </c>
-      <c r="E39" s="12" t="s">
-        <v>216</v>
+        <v>202</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -4301,166 +4276,166 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView zoomScale="164" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="10" customFormat="1" ht="24" customHeight="1">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:3" s="9" customFormat="1" ht="24" customHeight="1">
+      <c r="A1" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="16">
+      <c r="C1" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="16">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="16">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="16">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="16">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="16">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
         <v>107</v>
       </c>
       <c r="B7" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="16">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
         <v>108</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="16">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B9" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="16">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B10" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="16">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B11" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="16">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="16">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B13" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="16">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C14" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="16">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B15" t="s">
+        <v>150</v>
+      </c>
+      <c r="C15" t="s">
         <v>151</v>
       </c>
-      <c r="C15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="16">
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B16" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="16">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -4475,14 +4450,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="19.83203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="51.33203125" style="3" customWidth="1"/>
@@ -4494,15 +4469,15 @@
     <col min="8" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="10" customFormat="1" ht="24" customHeight="1">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:3" s="9" customFormat="1" ht="24" customHeight="1">
+      <c r="A1" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>130</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -4510,7 +4485,7 @@
         <v>67</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -4518,7 +4493,7 @@
         <v>68</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -4526,7 +4501,7 @@
         <v>69</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -4534,7 +4509,7 @@
         <v>70</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -4542,7 +4517,7 @@
         <v>71</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -4550,7 +4525,7 @@
         <v>72</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -4558,7 +4533,7 @@
         <v>73</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -4574,7 +4549,7 @@
         <v>75</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -4582,7 +4557,7 @@
         <v>76</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -4590,7 +4565,7 @@
         <v>77</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -4598,10 +4573,10 @@
         <v>78</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -4609,7 +4584,7 @@
         <v>79</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>120</v>
+        <v>382</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -4617,7 +4592,7 @@
         <v>80</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -4625,7 +4600,7 @@
         <v>81</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -4636,7 +4611,7 @@
         <v>82</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -4644,10 +4619,10 @@
         <v>83</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -4655,10 +4630,10 @@
         <v>84</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -4666,14 +4641,14 @@
         <v>85</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="17">
-      <c r="B23" s="11"/>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="18">
+      <c r="B23" s="10"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="B25" s="7"/>
+      <c r="B25" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4686,14 +4661,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
@@ -4701,191 +4676,191 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="17">
+      <c r="C1" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18">
       <c r="A2" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" ht="18">
+      <c r="A3" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" ht="18">
+      <c r="A4" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:3" ht="17">
-      <c r="A3" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" ht="18">
+      <c r="A5" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:3" ht="17">
-      <c r="A4" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" ht="18">
+      <c r="A6" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="C4" s="3"/>
-    </row>
-    <row r="5" spans="1:3" ht="17">
-      <c r="A5" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>358</v>
-      </c>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:3" ht="17">
-      <c r="A6" s="2" t="s">
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" ht="18">
+      <c r="A7" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B7" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:3" ht="17">
-      <c r="A7" s="2" t="s">
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" ht="18">
+      <c r="A8" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:3" ht="17">
-      <c r="A8" s="2" t="s">
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:3" ht="18">
+      <c r="A9" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="C8" s="3"/>
-    </row>
-    <row r="9" spans="1:3" ht="17">
-      <c r="A9" s="2" t="s">
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:3" ht="18">
+      <c r="A10" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="C9" s="3"/>
-    </row>
-    <row r="10" spans="1:3" ht="17">
-      <c r="A10" s="2" t="s">
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:3" ht="18">
+      <c r="A11" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:3" ht="17">
-      <c r="A11" s="2" t="s">
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:3" ht="18">
+      <c r="A12" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B12" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:3" ht="17">
-      <c r="A12" s="2" t="s">
+      <c r="C12" s="3" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="18">
+      <c r="A13" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B13" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="18">
+      <c r="A14" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>365</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="17">
-      <c r="A13" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>365</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="17">
-      <c r="A14" s="2" t="s">
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:3" ht="18">
+      <c r="A15" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B15" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="1:3" ht="17">
-      <c r="A15" s="2" t="s">
+      <c r="C15" s="3"/>
+    </row>
+    <row r="16" spans="1:3" ht="18">
+      <c r="A16" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>367</v>
       </c>
-      <c r="C15" s="3"/>
-    </row>
-    <row r="16" spans="1:3" ht="17">
-      <c r="A16" s="2" t="s">
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="1:3" ht="18">
+      <c r="A17" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B17" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="1:3" ht="18">
+      <c r="A18" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:3" ht="18">
+      <c r="A19" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>368</v>
       </c>
-      <c r="C16" s="3"/>
-    </row>
-    <row r="17" spans="1:3" ht="17">
-      <c r="A17" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>368</v>
-      </c>
-      <c r="C17" s="3"/>
-    </row>
-    <row r="18" spans="1:3" ht="17">
-      <c r="A18" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>368</v>
-      </c>
-      <c r="C18" s="3"/>
-    </row>
-    <row r="19" spans="1:3" ht="17">
-      <c r="A19" s="2" t="s">
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:3" ht="18">
+      <c r="A20" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="C19" s="3"/>
-    </row>
-    <row r="20" spans="1:3" ht="17">
-      <c r="A20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>355</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -4899,14 +4874,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="16.1640625" customWidth="1"/>
     <col min="2" max="2" width="24.6640625" customWidth="1"/>
@@ -4915,365 +4890,365 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C1" t="s">
         <v>223</v>
-      </c>
-      <c r="C1" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B2" t="s">
         <v>225</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>226</v>
-      </c>
-      <c r="C2" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
+        <v>227</v>
+      </c>
+      <c r="B3" t="s">
         <v>228</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>229</v>
-      </c>
-      <c r="C3" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
+        <v>230</v>
+      </c>
+      <c r="B4" t="s">
         <v>231</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>232</v>
-      </c>
-      <c r="C4" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B5" t="s">
         <v>234</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>235</v>
-      </c>
-      <c r="C5" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
+        <v>236</v>
+      </c>
+      <c r="B6" t="s">
         <v>237</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>238</v>
-      </c>
-      <c r="C6" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
+        <v>239</v>
+      </c>
+      <c r="B7" t="s">
         <v>240</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>241</v>
-      </c>
-      <c r="C7" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B8" t="s">
+        <v>240</v>
+      </c>
+      <c r="C8" t="s">
         <v>241</v>
-      </c>
-      <c r="C8" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B9" t="s">
+        <v>240</v>
+      </c>
+      <c r="C9" t="s">
         <v>241</v>
-      </c>
-      <c r="C9" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
+        <v>244</v>
+      </c>
+      <c r="B10" t="s">
         <v>245</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>246</v>
-      </c>
-      <c r="C10" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B11" t="s">
+        <v>240</v>
+      </c>
+      <c r="C11" t="s">
         <v>241</v>
-      </c>
-      <c r="C11" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
+        <v>248</v>
+      </c>
+      <c r="B12" t="s">
         <v>249</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>250</v>
-      </c>
-      <c r="C12" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
+        <v>251</v>
+      </c>
+      <c r="B13" t="s">
         <v>252</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>253</v>
-      </c>
-      <c r="C13" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
+        <v>254</v>
+      </c>
+      <c r="B14" t="s">
         <v>255</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>256</v>
-      </c>
-      <c r="C14" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
+        <v>257</v>
+      </c>
+      <c r="B15" t="s">
         <v>258</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>259</v>
-      </c>
-      <c r="C15" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
+        <v>260</v>
+      </c>
+      <c r="B16" t="s">
         <v>261</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>262</v>
-      </c>
-      <c r="C16" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B17" t="s">
+        <v>261</v>
+      </c>
+      <c r="C17" t="s">
         <v>262</v>
-      </c>
-      <c r="C17" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B18" t="s">
+        <v>261</v>
+      </c>
+      <c r="C18" t="s">
         <v>262</v>
-      </c>
-      <c r="C18" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B19" t="s">
+        <v>249</v>
+      </c>
+      <c r="C19" t="s">
         <v>250</v>
-      </c>
-      <c r="C19" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
+        <v>266</v>
+      </c>
+      <c r="B20" t="s">
         <v>267</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>268</v>
-      </c>
-      <c r="C20" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
+        <v>269</v>
+      </c>
+      <c r="B21" t="s">
         <v>270</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" s="4" t="s">
         <v>271</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
+        <v>272</v>
+      </c>
+      <c r="B22" t="s">
         <v>273</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" s="4" t="s">
         <v>274</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
+        <v>275</v>
+      </c>
+      <c r="B23" t="s">
         <v>276</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" s="4" t="s">
         <v>277</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
+        <v>278</v>
+      </c>
+      <c r="B24" t="s">
         <v>279</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" s="4" t="s">
         <v>280</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
+        <v>281</v>
+      </c>
+      <c r="B25" t="s">
         <v>282</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" s="4" t="s">
         <v>283</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B26" t="s">
+        <v>231</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>232</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
+        <v>285</v>
+      </c>
+      <c r="B27" t="s">
         <v>286</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" s="4" t="s">
         <v>287</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
+        <v>288</v>
+      </c>
+      <c r="B28" t="s">
         <v>289</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" s="4" t="s">
         <v>290</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
+        <v>291</v>
+      </c>
+      <c r="B29" t="s">
         <v>292</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" s="4" t="s">
         <v>293</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B30" t="s">
+        <v>286</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>287</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
+        <v>295</v>
+      </c>
+      <c r="B31" t="s">
         <v>296</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" s="4" t="s">
         <v>297</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B32" t="s">
+        <v>282</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>283</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B33" t="s">
+        <v>249</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>250</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -5288,14 +5263,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="125" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="23.83203125" customWidth="1"/>
     <col min="2" max="2" width="50.5" customWidth="1"/>
@@ -5303,15 +5278,15 @@
     <col min="5" max="5" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="9" customFormat="1" ht="24" customHeight="1">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:5" s="8" customFormat="1" ht="24" customHeight="1">
+      <c r="A1" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>130</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -5319,10 +5294,10 @@
         <v>86</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -5330,7 +5305,7 @@
         <v>60</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C3" s="3"/>
     </row>
@@ -5339,7 +5314,7 @@
         <v>87</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C4" s="3"/>
     </row>
@@ -5348,7 +5323,7 @@
         <v>88</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C5" s="3"/>
     </row>
@@ -5357,17 +5332,17 @@
         <v>89</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="E6" s="7"/>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="3" t="s">
         <v>90</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C7" s="3"/>
     </row>
@@ -5376,7 +5351,7 @@
         <v>91</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C8" s="3"/>
     </row>
@@ -5385,7 +5360,7 @@
         <v>92</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C9" s="3"/>
     </row>
@@ -5394,7 +5369,7 @@
         <v>93</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C10" s="3"/>
     </row>
@@ -5403,7 +5378,7 @@
         <v>94</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C11" s="3"/>
     </row>
@@ -5412,7 +5387,7 @@
         <v>95</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C12" s="3"/>
     </row>
@@ -5421,7 +5396,7 @@
         <v>96</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C13" s="3"/>
     </row>
@@ -5429,8 +5404,8 @@
       <c r="A14" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>324</v>
+      <c r="B14" s="5" t="s">
+        <v>323</v>
       </c>
       <c r="C14" s="3"/>
     </row>
@@ -5438,8 +5413,8 @@
       <c r="A15" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>332</v>
+      <c r="B15" s="5" t="s">
+        <v>331</v>
       </c>
       <c r="C15" s="3"/>
     </row>
@@ -5448,10 +5423,10 @@
         <v>99</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -5459,7 +5434,7 @@
         <v>100</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C17" s="3"/>
     </row>
@@ -5468,10 +5443,10 @@
         <v>101</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -5479,7 +5454,7 @@
         <v>102</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C19" s="3"/>
     </row>
@@ -5488,7 +5463,7 @@
         <v>103</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C20" s="3"/>
     </row>
@@ -5497,10 +5472,10 @@
         <v>104</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -5508,10 +5483,10 @@
         <v>105</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -5519,10 +5494,10 @@
         <v>106</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>